<commit_message>
EPBDS-7799 Fix NPE in unary + and - operators
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/Arithmetic.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/Arithmetic.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="16935" windowHeight="7185"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="16935" windowHeight="7185" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Operators" sheetId="12" r:id="rId1"/>
@@ -13,13 +13,14 @@
     <sheet name="Mul" sheetId="16" r:id="rId4"/>
     <sheet name="Div" sheetId="17" r:id="rId5"/>
     <sheet name="Pow" sheetId="18" r:id="rId6"/>
+    <sheet name="unary" sheetId="19" r:id="rId7"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3892" uniqueCount="624">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3966" uniqueCount="629">
   <si>
     <t>Result</t>
   </si>
@@ -1892,6 +1893,21 @@
   <si>
     <t>_res_.$v$divide2 (34)</t>
   </si>
+  <si>
+    <t>neg</t>
+  </si>
+  <si>
+    <t>pos</t>
+  </si>
+  <si>
+    <t>Spreadsheet SpreadsheetResult unary (long v1, double v2, Long v3, Double v4, BigInteger v5, BigDecimal v6)</t>
+  </si>
+  <si>
+    <t>Test unary negTest</t>
+  </si>
+  <si>
+    <t>Test unary posTest</t>
+  </si>
 </sst>
 </file>
 
@@ -2452,7 +2468,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2462,8 +2478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:L90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="H71" sqref="H71"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2583,6 +2599,9 @@
       <c r="J10">
         <v>0.66666666666666596</v>
       </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B11" s="57"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B12" s="87"/>
@@ -18639,14 +18658,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="C104:H104"/>
-    <mergeCell ref="C112:H112"/>
-    <mergeCell ref="C184:H184"/>
-    <mergeCell ref="C144:H144"/>
-    <mergeCell ref="C152:H152"/>
-    <mergeCell ref="C160:H160"/>
-    <mergeCell ref="C168:H168"/>
-    <mergeCell ref="C176:H176"/>
     <mergeCell ref="C200:H200"/>
     <mergeCell ref="C208:H208"/>
     <mergeCell ref="C64:H64"/>
@@ -18663,6 +18674,14 @@
     <mergeCell ref="C128:H128"/>
     <mergeCell ref="C88:H88"/>
     <mergeCell ref="C96:H96"/>
+    <mergeCell ref="C104:H104"/>
+    <mergeCell ref="C112:H112"/>
+    <mergeCell ref="C184:H184"/>
+    <mergeCell ref="C144:H144"/>
+    <mergeCell ref="C152:H152"/>
+    <mergeCell ref="C160:H160"/>
+    <mergeCell ref="C168:H168"/>
+    <mergeCell ref="C176:H176"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -33275,14 +33294,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="C184:H184"/>
-    <mergeCell ref="C136:H136"/>
-    <mergeCell ref="C120:H120"/>
-    <mergeCell ref="C144:H144"/>
-    <mergeCell ref="C152:H152"/>
-    <mergeCell ref="C160:H160"/>
-    <mergeCell ref="C168:H168"/>
-    <mergeCell ref="C176:H176"/>
     <mergeCell ref="C200:H200"/>
     <mergeCell ref="C208:H208"/>
     <mergeCell ref="H3:M3"/>
@@ -33299,6 +33310,14 @@
     <mergeCell ref="C56:H56"/>
     <mergeCell ref="C112:H112"/>
     <mergeCell ref="C128:H128"/>
+    <mergeCell ref="C184:H184"/>
+    <mergeCell ref="C136:H136"/>
+    <mergeCell ref="C120:H120"/>
+    <mergeCell ref="C144:H144"/>
+    <mergeCell ref="C152:H152"/>
+    <mergeCell ref="C160:H160"/>
+    <mergeCell ref="C168:H168"/>
+    <mergeCell ref="C176:H176"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -48102,6 +48121,16 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="H3:M3"/>
+    <mergeCell ref="C32:H32"/>
+    <mergeCell ref="C40:H40"/>
+    <mergeCell ref="C88:H88"/>
+    <mergeCell ref="C96:H96"/>
+    <mergeCell ref="C80:H80"/>
+    <mergeCell ref="C48:H48"/>
+    <mergeCell ref="C56:H56"/>
+    <mergeCell ref="C64:H64"/>
+    <mergeCell ref="C72:H72"/>
     <mergeCell ref="C200:H200"/>
     <mergeCell ref="C208:H208"/>
     <mergeCell ref="C104:H104"/>
@@ -48116,16 +48145,6 @@
     <mergeCell ref="C160:H160"/>
     <mergeCell ref="C168:H168"/>
     <mergeCell ref="C120:H120"/>
-    <mergeCell ref="H3:M3"/>
-    <mergeCell ref="C32:H32"/>
-    <mergeCell ref="C40:H40"/>
-    <mergeCell ref="C88:H88"/>
-    <mergeCell ref="C96:H96"/>
-    <mergeCell ref="C80:H80"/>
-    <mergeCell ref="C48:H48"/>
-    <mergeCell ref="C56:H56"/>
-    <mergeCell ref="C64:H64"/>
-    <mergeCell ref="C72:H72"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -63027,20 +63046,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="B219:G219"/>
-    <mergeCell ref="C200:H200"/>
-    <mergeCell ref="C208:H208"/>
-    <mergeCell ref="C152:H152"/>
-    <mergeCell ref="C160:H160"/>
-    <mergeCell ref="C168:H168"/>
-    <mergeCell ref="C176:H176"/>
-    <mergeCell ref="C184:H184"/>
-    <mergeCell ref="C192:H192"/>
-    <mergeCell ref="H3:M3"/>
-    <mergeCell ref="C32:H32"/>
-    <mergeCell ref="C40:H40"/>
-    <mergeCell ref="C48:H48"/>
-    <mergeCell ref="C56:H56"/>
     <mergeCell ref="C144:H144"/>
     <mergeCell ref="C136:H136"/>
     <mergeCell ref="C128:H128"/>
@@ -63051,6 +63056,20 @@
     <mergeCell ref="C88:H88"/>
     <mergeCell ref="C96:H96"/>
     <mergeCell ref="C104:H104"/>
+    <mergeCell ref="H3:M3"/>
+    <mergeCell ref="C32:H32"/>
+    <mergeCell ref="C40:H40"/>
+    <mergeCell ref="C48:H48"/>
+    <mergeCell ref="C56:H56"/>
+    <mergeCell ref="B219:G219"/>
+    <mergeCell ref="C200:H200"/>
+    <mergeCell ref="C208:H208"/>
+    <mergeCell ref="C152:H152"/>
+    <mergeCell ref="C160:H160"/>
+    <mergeCell ref="C168:H168"/>
+    <mergeCell ref="C176:H176"/>
+    <mergeCell ref="C184:H184"/>
+    <mergeCell ref="C192:H192"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -65925,4 +65944,1345 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:AF27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8.5703125" style="56" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="2.140625" style="56" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8.42578125" style="56" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="6.42578125" style="56" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="5" style="56" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="6.7109375" style="56" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="5.7109375" style="56" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="7" style="56" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="10" width="18.42578125" style="56" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="13" width="17.85546875" style="56" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="18.42578125" style="56" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="16" width="18.7109375" style="56" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="17.85546875" style="56" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="18.42578125" style="56" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="18.5703125" style="56" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="18.7109375" style="56" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="19.140625" style="56" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="24" width="20" style="56" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="19.140625" style="56" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="19.7109375" style="56" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="19.85546875" style="56" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="20" style="56" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="20.42578125" style="56" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="21.42578125" style="56" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="9.140625" style="56" collapsed="1"/>
+    <col min="32" max="32" width="9.140625" style="56"/>
+    <col min="33" max="16384" width="9.140625" style="56" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:31" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H3" s="90" t="s">
+        <v>626</v>
+      </c>
+      <c r="I3" s="90"/>
+      <c r="J3" s="90"/>
+      <c r="K3" s="90"/>
+      <c r="L3" s="90"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
+      <c r="Y3" s="8"/>
+      <c r="Z3" s="8"/>
+      <c r="AA3" s="8"/>
+      <c r="AB3" s="8"/>
+      <c r="AC3" s="8"/>
+      <c r="AD3" s="8"/>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="H4" s="6"/>
+      <c r="I4" s="56" t="s">
+        <v>123</v>
+      </c>
+      <c r="J4" s="56" t="s">
+        <v>124</v>
+      </c>
+      <c r="K4" s="56" t="s">
+        <v>125</v>
+      </c>
+      <c r="L4" s="56" t="s">
+        <v>126</v>
+      </c>
+      <c r="M4" s="56" t="s">
+        <v>127</v>
+      </c>
+      <c r="N4" s="56" t="s">
+        <v>128</v>
+      </c>
+      <c r="O4" s="56" t="s">
+        <v>129</v>
+      </c>
+      <c r="P4" s="56" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q4" s="56" t="s">
+        <v>131</v>
+      </c>
+      <c r="R4" s="56" t="s">
+        <v>132</v>
+      </c>
+      <c r="S4" s="56" t="s">
+        <v>133</v>
+      </c>
+      <c r="T4" s="56" t="s">
+        <v>134</v>
+      </c>
+      <c r="U4" s="56" t="s">
+        <v>141</v>
+      </c>
+      <c r="V4" s="56" t="s">
+        <v>143</v>
+      </c>
+      <c r="W4" s="56" t="s">
+        <v>135</v>
+      </c>
+      <c r="X4" s="56" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y4" s="56" t="s">
+        <v>137</v>
+      </c>
+      <c r="Z4" s="56" t="s">
+        <v>138</v>
+      </c>
+      <c r="AA4" s="56" t="s">
+        <v>139</v>
+      </c>
+      <c r="AB4" s="56" t="s">
+        <v>140</v>
+      </c>
+      <c r="AC4" s="56" t="s">
+        <v>142</v>
+      </c>
+      <c r="AD4" s="56" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="H5" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="O5" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="P5" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q5" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="R5" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="S5" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="T5" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="U5" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="V5" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="W5" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="X5" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y5" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="Z5" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="AA5" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="AB5" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="AC5" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="AD5" s="6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="H6" s="56" t="s">
+        <v>624</v>
+      </c>
+      <c r="I6" s="7" t="str">
+        <f>"=-$Y"</f>
+        <v>=-$Y</v>
+      </c>
+      <c r="J6" s="7" t="str">
+        <f t="shared" ref="J6:AD6" si="0">"=-$Y"</f>
+        <v>=-$Y</v>
+      </c>
+      <c r="K6" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>=-$Y</v>
+      </c>
+      <c r="L6" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>=-$Y</v>
+      </c>
+      <c r="M6" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>=-$Y</v>
+      </c>
+      <c r="N6" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>=-$Y</v>
+      </c>
+      <c r="O6" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>=-$Y</v>
+      </c>
+      <c r="P6" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>=-$Y</v>
+      </c>
+      <c r="Q6" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>=-$Y</v>
+      </c>
+      <c r="R6" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>=-$Y</v>
+      </c>
+      <c r="S6" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>=-$Y</v>
+      </c>
+      <c r="T6" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>=-$Y</v>
+      </c>
+      <c r="U6" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>=-$Y</v>
+      </c>
+      <c r="V6" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>=-$Y</v>
+      </c>
+      <c r="W6" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>=-$Y</v>
+      </c>
+      <c r="X6" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>=-$Y</v>
+      </c>
+      <c r="Y6" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>=-$Y</v>
+      </c>
+      <c r="Z6" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>=-$Y</v>
+      </c>
+      <c r="AA6" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>=-$Y</v>
+      </c>
+      <c r="AB6" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>=-$Y</v>
+      </c>
+      <c r="AC6" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>=-$Y</v>
+      </c>
+      <c r="AD6" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>=-$Y</v>
+      </c>
+      <c r="AE6" s="7"/>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="H7" s="56" t="s">
+        <v>625</v>
+      </c>
+      <c r="I7" s="7" t="str">
+        <f>"=+$Y"</f>
+        <v>=+$Y</v>
+      </c>
+      <c r="J7" s="7" t="str">
+        <f t="shared" ref="J7:AD7" si="1">"=+$Y"</f>
+        <v>=+$Y</v>
+      </c>
+      <c r="K7" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>=+$Y</v>
+      </c>
+      <c r="L7" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>=+$Y</v>
+      </c>
+      <c r="M7" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>=+$Y</v>
+      </c>
+      <c r="N7" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>=+$Y</v>
+      </c>
+      <c r="O7" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>=+$Y</v>
+      </c>
+      <c r="P7" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>=+$Y</v>
+      </c>
+      <c r="Q7" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>=+$Y</v>
+      </c>
+      <c r="R7" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>=+$Y</v>
+      </c>
+      <c r="S7" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>=+$Y</v>
+      </c>
+      <c r="T7" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>=+$Y</v>
+      </c>
+      <c r="U7" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>=+$Y</v>
+      </c>
+      <c r="V7" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>=+$Y</v>
+      </c>
+      <c r="W7" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>=+$Y</v>
+      </c>
+      <c r="X7" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>=+$Y</v>
+      </c>
+      <c r="Y7" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>=+$Y</v>
+      </c>
+      <c r="Z7" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>=+$Y</v>
+      </c>
+      <c r="AA7" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>=+$Y</v>
+      </c>
+      <c r="AB7" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>=+$Y</v>
+      </c>
+      <c r="AC7" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>=+$Y</v>
+      </c>
+      <c r="AD7" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>=+$Y</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="C12" s="89" t="s">
+        <v>627</v>
+      </c>
+      <c r="D12" s="89"/>
+      <c r="E12" s="89"/>
+      <c r="F12" s="89"/>
+      <c r="G12" s="89"/>
+      <c r="H12" s="89"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="9"/>
+      <c r="R12" s="9"/>
+      <c r="S12" s="9"/>
+      <c r="T12" s="9"/>
+      <c r="U12" s="9"/>
+      <c r="V12" s="9"/>
+      <c r="W12" s="9"/>
+      <c r="X12" s="9"/>
+      <c r="Y12" s="9"/>
+      <c r="Z12" s="9"/>
+      <c r="AA12" s="9"/>
+      <c r="AB12" s="9"/>
+      <c r="AC12" s="9"/>
+      <c r="AD12" s="9"/>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="C13" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="I13" s="9" t="str">
+        <f>"_res_.$"&amp;I$4&amp;"$neg"</f>
+        <v>_res_.$b2$neg</v>
+      </c>
+      <c r="J13" s="9" t="str">
+        <f t="shared" ref="J13:AD13" si="2">"_res_.$"&amp;J$4&amp;"$neg"</f>
+        <v>_res_.$s2$neg</v>
+      </c>
+      <c r="K13" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>_res_.$i2$neg</v>
+      </c>
+      <c r="L13" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>_res_.$l2$neg</v>
+      </c>
+      <c r="M13" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>_res_.$f2$neg</v>
+      </c>
+      <c r="N13" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>_res_.$d2$neg</v>
+      </c>
+      <c r="O13" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>_res_.$B2$neg</v>
+      </c>
+      <c r="P13" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>_res_.$S2$neg</v>
+      </c>
+      <c r="Q13" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>_res_.$I2$neg</v>
+      </c>
+      <c r="R13" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>_res_.$L2$neg</v>
+      </c>
+      <c r="S13" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>_res_.$F2$neg</v>
+      </c>
+      <c r="T13" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>_res_.$D2$neg</v>
+      </c>
+      <c r="U13" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>_res_.$BI2$neg</v>
+      </c>
+      <c r="V13" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>_res_.$BD2$neg</v>
+      </c>
+      <c r="W13" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>_res_.$BV2$neg</v>
+      </c>
+      <c r="X13" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>_res_.$SV2$neg</v>
+      </c>
+      <c r="Y13" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>_res_.$IV2$neg</v>
+      </c>
+      <c r="Z13" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>_res_.$LV2$neg</v>
+      </c>
+      <c r="AA13" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>_res_.$FV2$neg</v>
+      </c>
+      <c r="AB13" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>_res_.$DV2$neg</v>
+      </c>
+      <c r="AC13" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>_res_.$BIV2$neg</v>
+      </c>
+      <c r="AD13" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>_res_.$BDV2$neg</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="C14" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="I14" s="9" t="str">
+        <f t="shared" ref="I14:AD14" si="3">I$4</f>
+        <v>b2</v>
+      </c>
+      <c r="J14" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>s2</v>
+      </c>
+      <c r="K14" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>i2</v>
+      </c>
+      <c r="L14" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>l2</v>
+      </c>
+      <c r="M14" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>f2</v>
+      </c>
+      <c r="N14" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>d2</v>
+      </c>
+      <c r="O14" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>B2</v>
+      </c>
+      <c r="P14" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>S2</v>
+      </c>
+      <c r="Q14" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>I2</v>
+      </c>
+      <c r="R14" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>L2</v>
+      </c>
+      <c r="S14" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>F2</v>
+      </c>
+      <c r="T14" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>D2</v>
+      </c>
+      <c r="U14" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>BI2</v>
+      </c>
+      <c r="V14" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>BD2</v>
+      </c>
+      <c r="W14" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>BV2</v>
+      </c>
+      <c r="X14" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>SV2</v>
+      </c>
+      <c r="Y14" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>IV2</v>
+      </c>
+      <c r="Z14" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>LV2</v>
+      </c>
+      <c r="AA14" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>FV2</v>
+      </c>
+      <c r="AB14" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>DV2</v>
+      </c>
+      <c r="AC14" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>BIV2</v>
+      </c>
+      <c r="AD14" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>BDV2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="C15" s="9">
+        <v>3</v>
+      </c>
+      <c r="D15" s="9">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E15" s="9">
+        <v>34</v>
+      </c>
+      <c r="F15" s="9">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="G15" s="9">
+        <v>67</v>
+      </c>
+      <c r="H15" s="9">
+        <v>13.65</v>
+      </c>
+      <c r="I15" s="9">
+        <v>-3</v>
+      </c>
+      <c r="J15" s="9">
+        <v>-3</v>
+      </c>
+      <c r="K15" s="9">
+        <v>-3</v>
+      </c>
+      <c r="L15" s="9">
+        <v>-3</v>
+      </c>
+      <c r="M15" s="9">
+        <v>-2.2999999999999998</v>
+      </c>
+      <c r="N15" s="9">
+        <v>-2.2999999999999998</v>
+      </c>
+      <c r="O15" s="9">
+        <v>-34</v>
+      </c>
+      <c r="P15" s="9">
+        <v>-34</v>
+      </c>
+      <c r="Q15" s="9">
+        <v>-34</v>
+      </c>
+      <c r="R15" s="9">
+        <v>-34</v>
+      </c>
+      <c r="S15" s="9">
+        <v>-17.600000000000001</v>
+      </c>
+      <c r="T15" s="9">
+        <v>-17.600000000000001</v>
+      </c>
+      <c r="U15" s="9">
+        <v>-67</v>
+      </c>
+      <c r="V15" s="9">
+        <v>-13.65</v>
+      </c>
+      <c r="W15" s="9">
+        <v>-34</v>
+      </c>
+      <c r="X15" s="9">
+        <v>-34</v>
+      </c>
+      <c r="Y15" s="9">
+        <v>-34</v>
+      </c>
+      <c r="Z15" s="9">
+        <v>-34</v>
+      </c>
+      <c r="AA15" s="9">
+        <v>-17.600000000000001</v>
+      </c>
+      <c r="AB15" s="9">
+        <v>-17.600000000000001</v>
+      </c>
+      <c r="AC15" s="9">
+        <v>-67</v>
+      </c>
+      <c r="AD15" s="9">
+        <v>-13.65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="C16" s="9">
+        <v>-3</v>
+      </c>
+      <c r="D16" s="9">
+        <v>-2.2999999999999998</v>
+      </c>
+      <c r="E16" s="9">
+        <v>-34</v>
+      </c>
+      <c r="F16" s="9">
+        <v>-17.600000000000001</v>
+      </c>
+      <c r="G16" s="9">
+        <v>-67</v>
+      </c>
+      <c r="H16" s="9">
+        <v>-13.65</v>
+      </c>
+      <c r="I16" s="9">
+        <v>3</v>
+      </c>
+      <c r="J16" s="9">
+        <v>3</v>
+      </c>
+      <c r="K16" s="9">
+        <v>3</v>
+      </c>
+      <c r="L16" s="9">
+        <v>3</v>
+      </c>
+      <c r="M16" s="9">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="N16" s="9">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="O16" s="9">
+        <v>34</v>
+      </c>
+      <c r="P16" s="9">
+        <v>34</v>
+      </c>
+      <c r="Q16" s="9">
+        <v>34</v>
+      </c>
+      <c r="R16" s="9">
+        <v>34</v>
+      </c>
+      <c r="S16" s="9">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="T16" s="9">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="U16" s="9">
+        <v>67</v>
+      </c>
+      <c r="V16" s="9">
+        <v>13.65</v>
+      </c>
+      <c r="W16" s="9">
+        <v>34</v>
+      </c>
+      <c r="X16" s="9">
+        <v>34</v>
+      </c>
+      <c r="Y16" s="9">
+        <v>34</v>
+      </c>
+      <c r="Z16" s="9">
+        <v>34</v>
+      </c>
+      <c r="AA16" s="9">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="AB16" s="9">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="AC16" s="9">
+        <v>67</v>
+      </c>
+      <c r="AD16" s="9">
+        <v>13.65</v>
+      </c>
+    </row>
+    <row r="17" spans="3:30" x14ac:dyDescent="0.2">
+      <c r="C17" s="9">
+        <v>0</v>
+      </c>
+      <c r="D17" s="9">
+        <v>0</v>
+      </c>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9">
+        <v>0</v>
+      </c>
+      <c r="J17" s="9">
+        <v>0</v>
+      </c>
+      <c r="K17" s="9">
+        <v>0</v>
+      </c>
+      <c r="L17" s="9">
+        <v>0</v>
+      </c>
+      <c r="M17" s="9">
+        <v>0</v>
+      </c>
+      <c r="N17" s="9">
+        <v>0</v>
+      </c>
+      <c r="O17" s="9"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="9"/>
+      <c r="R17" s="9"/>
+      <c r="S17" s="9"/>
+      <c r="T17" s="9"/>
+      <c r="U17" s="9"/>
+      <c r="V17" s="9"/>
+      <c r="W17" s="9"/>
+      <c r="X17" s="9"/>
+      <c r="Y17" s="9"/>
+      <c r="Z17" s="9"/>
+      <c r="AA17" s="9"/>
+      <c r="AB17" s="9"/>
+      <c r="AC17" s="9"/>
+      <c r="AD17" s="9"/>
+    </row>
+    <row r="22" spans="3:30" x14ac:dyDescent="0.2">
+      <c r="C22" s="89" t="s">
+        <v>628</v>
+      </c>
+      <c r="D22" s="89"/>
+      <c r="E22" s="89"/>
+      <c r="F22" s="89"/>
+      <c r="G22" s="89"/>
+      <c r="H22" s="89"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
+      <c r="P22" s="9"/>
+      <c r="Q22" s="9"/>
+      <c r="R22" s="9"/>
+      <c r="S22" s="9"/>
+      <c r="T22" s="9"/>
+      <c r="U22" s="9"/>
+      <c r="V22" s="9"/>
+      <c r="W22" s="9"/>
+      <c r="X22" s="9"/>
+      <c r="Y22" s="9"/>
+      <c r="Z22" s="9"/>
+      <c r="AA22" s="9"/>
+      <c r="AB22" s="9"/>
+      <c r="AC22" s="9"/>
+      <c r="AD22" s="9"/>
+    </row>
+    <row r="23" spans="3:30" x14ac:dyDescent="0.2">
+      <c r="C23" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="H23" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="I23" s="9" t="str">
+        <f>"_res_.$"&amp;I$4&amp;"$pos"</f>
+        <v>_res_.$b2$pos</v>
+      </c>
+      <c r="J23" s="9" t="str">
+        <f t="shared" ref="J23:AD23" si="4">"_res_.$"&amp;J$4&amp;"$pos"</f>
+        <v>_res_.$s2$pos</v>
+      </c>
+      <c r="K23" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>_res_.$i2$pos</v>
+      </c>
+      <c r="L23" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>_res_.$l2$pos</v>
+      </c>
+      <c r="M23" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>_res_.$f2$pos</v>
+      </c>
+      <c r="N23" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>_res_.$d2$pos</v>
+      </c>
+      <c r="O23" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>_res_.$B2$pos</v>
+      </c>
+      <c r="P23" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>_res_.$S2$pos</v>
+      </c>
+      <c r="Q23" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>_res_.$I2$pos</v>
+      </c>
+      <c r="R23" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>_res_.$L2$pos</v>
+      </c>
+      <c r="S23" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>_res_.$F2$pos</v>
+      </c>
+      <c r="T23" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>_res_.$D2$pos</v>
+      </c>
+      <c r="U23" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>_res_.$BI2$pos</v>
+      </c>
+      <c r="V23" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>_res_.$BD2$pos</v>
+      </c>
+      <c r="W23" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>_res_.$BV2$pos</v>
+      </c>
+      <c r="X23" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>_res_.$SV2$pos</v>
+      </c>
+      <c r="Y23" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>_res_.$IV2$pos</v>
+      </c>
+      <c r="Z23" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>_res_.$LV2$pos</v>
+      </c>
+      <c r="AA23" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>_res_.$FV2$pos</v>
+      </c>
+      <c r="AB23" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>_res_.$DV2$pos</v>
+      </c>
+      <c r="AC23" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>_res_.$BIV2$pos</v>
+      </c>
+      <c r="AD23" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>_res_.$BDV2$pos</v>
+      </c>
+    </row>
+    <row r="24" spans="3:30" x14ac:dyDescent="0.2">
+      <c r="C24" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="I24" s="9" t="str">
+        <f t="shared" ref="I24:AD24" si="5">I$4</f>
+        <v>b2</v>
+      </c>
+      <c r="J24" s="9" t="str">
+        <f t="shared" si="5"/>
+        <v>s2</v>
+      </c>
+      <c r="K24" s="9" t="str">
+        <f t="shared" si="5"/>
+        <v>i2</v>
+      </c>
+      <c r="L24" s="9" t="str">
+        <f t="shared" si="5"/>
+        <v>l2</v>
+      </c>
+      <c r="M24" s="9" t="str">
+        <f t="shared" si="5"/>
+        <v>f2</v>
+      </c>
+      <c r="N24" s="9" t="str">
+        <f t="shared" si="5"/>
+        <v>d2</v>
+      </c>
+      <c r="O24" s="9" t="str">
+        <f t="shared" si="5"/>
+        <v>B2</v>
+      </c>
+      <c r="P24" s="9" t="str">
+        <f t="shared" si="5"/>
+        <v>S2</v>
+      </c>
+      <c r="Q24" s="9" t="str">
+        <f t="shared" si="5"/>
+        <v>I2</v>
+      </c>
+      <c r="R24" s="9" t="str">
+        <f t="shared" si="5"/>
+        <v>L2</v>
+      </c>
+      <c r="S24" s="9" t="str">
+        <f t="shared" si="5"/>
+        <v>F2</v>
+      </c>
+      <c r="T24" s="9" t="str">
+        <f t="shared" si="5"/>
+        <v>D2</v>
+      </c>
+      <c r="U24" s="9" t="str">
+        <f t="shared" si="5"/>
+        <v>BI2</v>
+      </c>
+      <c r="V24" s="9" t="str">
+        <f t="shared" si="5"/>
+        <v>BD2</v>
+      </c>
+      <c r="W24" s="9" t="str">
+        <f t="shared" si="5"/>
+        <v>BV2</v>
+      </c>
+      <c r="X24" s="9" t="str">
+        <f t="shared" si="5"/>
+        <v>SV2</v>
+      </c>
+      <c r="Y24" s="9" t="str">
+        <f t="shared" si="5"/>
+        <v>IV2</v>
+      </c>
+      <c r="Z24" s="9" t="str">
+        <f t="shared" si="5"/>
+        <v>LV2</v>
+      </c>
+      <c r="AA24" s="9" t="str">
+        <f t="shared" si="5"/>
+        <v>FV2</v>
+      </c>
+      <c r="AB24" s="9" t="str">
+        <f t="shared" si="5"/>
+        <v>DV2</v>
+      </c>
+      <c r="AC24" s="9" t="str">
+        <f t="shared" si="5"/>
+        <v>BIV2</v>
+      </c>
+      <c r="AD24" s="9" t="str">
+        <f t="shared" si="5"/>
+        <v>BDV2</v>
+      </c>
+    </row>
+    <row r="25" spans="3:30" x14ac:dyDescent="0.2">
+      <c r="C25" s="9">
+        <v>3</v>
+      </c>
+      <c r="D25" s="9">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E25" s="9">
+        <v>34</v>
+      </c>
+      <c r="F25" s="9">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="G25" s="9">
+        <v>67</v>
+      </c>
+      <c r="H25" s="9">
+        <v>13.65</v>
+      </c>
+      <c r="I25" s="9">
+        <v>3</v>
+      </c>
+      <c r="J25" s="9">
+        <v>3</v>
+      </c>
+      <c r="K25" s="9">
+        <v>3</v>
+      </c>
+      <c r="L25" s="9">
+        <v>3</v>
+      </c>
+      <c r="M25" s="9">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="N25" s="9">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="O25" s="9">
+        <v>34</v>
+      </c>
+      <c r="P25" s="9">
+        <v>34</v>
+      </c>
+      <c r="Q25" s="9">
+        <v>34</v>
+      </c>
+      <c r="R25" s="9">
+        <v>34</v>
+      </c>
+      <c r="S25" s="9">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="T25" s="9">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="U25" s="9">
+        <v>67</v>
+      </c>
+      <c r="V25" s="9">
+        <v>13.65</v>
+      </c>
+      <c r="W25" s="9">
+        <v>34</v>
+      </c>
+      <c r="X25" s="9">
+        <v>34</v>
+      </c>
+      <c r="Y25" s="9">
+        <v>34</v>
+      </c>
+      <c r="Z25" s="9">
+        <v>34</v>
+      </c>
+      <c r="AA25" s="9">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="AB25" s="9">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="AC25" s="9">
+        <v>67</v>
+      </c>
+      <c r="AD25" s="9">
+        <v>13.65</v>
+      </c>
+    </row>
+    <row r="26" spans="3:30" x14ac:dyDescent="0.2">
+      <c r="C26" s="9">
+        <v>-3</v>
+      </c>
+      <c r="D26" s="9">
+        <v>-2.2999999999999998</v>
+      </c>
+      <c r="E26" s="9">
+        <v>-34</v>
+      </c>
+      <c r="F26" s="9">
+        <v>-17.600000000000001</v>
+      </c>
+      <c r="G26" s="9">
+        <v>-67</v>
+      </c>
+      <c r="H26" s="9">
+        <v>-13.65</v>
+      </c>
+      <c r="I26" s="9">
+        <v>-3</v>
+      </c>
+      <c r="J26" s="9">
+        <v>-3</v>
+      </c>
+      <c r="K26" s="9">
+        <v>-3</v>
+      </c>
+      <c r="L26" s="9">
+        <v>-3</v>
+      </c>
+      <c r="M26" s="9">
+        <v>-2.2999999999999998</v>
+      </c>
+      <c r="N26" s="9">
+        <v>-2.2999999999999998</v>
+      </c>
+      <c r="O26" s="9">
+        <v>-34</v>
+      </c>
+      <c r="P26" s="9">
+        <v>-34</v>
+      </c>
+      <c r="Q26" s="9">
+        <v>-34</v>
+      </c>
+      <c r="R26" s="9">
+        <v>-34</v>
+      </c>
+      <c r="S26" s="9">
+        <v>-17.600000000000001</v>
+      </c>
+      <c r="T26" s="9">
+        <v>-17.600000000000001</v>
+      </c>
+      <c r="U26" s="9">
+        <v>-67</v>
+      </c>
+      <c r="V26" s="9">
+        <v>-13.65</v>
+      </c>
+      <c r="W26" s="9">
+        <v>-34</v>
+      </c>
+      <c r="X26" s="9">
+        <v>-34</v>
+      </c>
+      <c r="Y26" s="9">
+        <v>-34</v>
+      </c>
+      <c r="Z26" s="9">
+        <v>-34</v>
+      </c>
+      <c r="AA26" s="9">
+        <v>-17.600000000000001</v>
+      </c>
+      <c r="AB26" s="9">
+        <v>-17.600000000000001</v>
+      </c>
+      <c r="AC26" s="9">
+        <v>-67</v>
+      </c>
+      <c r="AD26" s="9">
+        <v>-13.65</v>
+      </c>
+    </row>
+    <row r="27" spans="3:30" x14ac:dyDescent="0.2">
+      <c r="C27" s="9">
+        <v>0</v>
+      </c>
+      <c r="D27" s="9">
+        <v>0</v>
+      </c>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9">
+        <v>0</v>
+      </c>
+      <c r="J27" s="9">
+        <v>0</v>
+      </c>
+      <c r="K27" s="9">
+        <v>0</v>
+      </c>
+      <c r="L27" s="9">
+        <v>0</v>
+      </c>
+      <c r="M27" s="9">
+        <v>0</v>
+      </c>
+      <c r="N27" s="9">
+        <v>0</v>
+      </c>
+      <c r="O27" s="9"/>
+      <c r="P27" s="9"/>
+      <c r="Q27" s="9"/>
+      <c r="R27" s="9"/>
+      <c r="S27" s="9"/>
+      <c r="T27" s="9"/>
+      <c r="U27" s="9"/>
+      <c r="V27" s="9"/>
+      <c r="W27" s="9"/>
+      <c r="X27" s="9"/>
+      <c r="Y27" s="9"/>
+      <c r="Z27" s="9"/>
+      <c r="AA27" s="9"/>
+      <c r="AB27" s="9"/>
+      <c r="AC27" s="9"/>
+      <c r="AD27" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="H3:L3"/>
+    <mergeCell ref="C12:H12"/>
+    <mergeCell ref="C22:H22"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>